<commit_message>
Topic Selection - added credit card fraud detection topic
</commit_message>
<xml_diff>
--- a/Notes/Anish - Topic Selection Research.xlsx
+++ b/Notes/Anish - Topic Selection Research.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Masters\MSc in Data Science\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DF7D1525-F745-48F6-A830-F97D1CC658E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A3937645-33FE-4A3D-B379-45B5B6246A10}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="0" windowWidth="19470" windowHeight="8130" activeTab="2" xr2:uid="{E21BDA22-B8EB-45F6-B92D-A3EF9FFC5147}"/>
+    <workbookView xWindow="3060" yWindow="0" windowWidth="19470" windowHeight="8130" xr2:uid="{E21BDA22-B8EB-45F6-B92D-A3EF9FFC5147}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Attrition in the Workforce" sheetId="1" r:id="rId1"/>
     <sheet name="2 - Churn in Telecos" sheetId="2" r:id="rId2"/>
-    <sheet name="3 - " sheetId="3" r:id="rId3"/>
-    <sheet name="Topic 4" sheetId="4" r:id="rId4"/>
+    <sheet name="3 - Credit Card Fraud Detection" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t xml:space="preserve">Title </t>
   </si>
@@ -36,13 +35,7 @@
     <t>Link to the Paper</t>
   </si>
   <si>
-    <t>Understanding of the Dataset</t>
-  </si>
-  <si>
     <t>Dataset Link</t>
-  </si>
-  <si>
-    <t>Understanding the Methodology Used</t>
   </si>
   <si>
     <t>Understanding of the Dataset/
@@ -138,6 +131,36 @@
   </si>
   <si>
     <t>Science Direct</t>
+  </si>
+  <si>
+    <t>Credit Card Fraud Detection - Machine Learning methods</t>
+  </si>
+  <si>
+    <t>Credit Card Fraud Detection - Machine Learning methods - IEEE Conference Publication</t>
+  </si>
+  <si>
+    <t>Credit card fraud detection using machine learning techniques: A comparative analysis - IEEE Conference Publication</t>
+  </si>
+  <si>
+    <t>Credit card fraud detection using machine learning techniques: A comparative analysis</t>
+  </si>
+  <si>
+    <t>Random forest for credit card fraud detection - IEEE Conference Publication</t>
+  </si>
+  <si>
+    <t>Random forest for credit card fraud detection</t>
+  </si>
+  <si>
+    <t>Combining unsupervised and supervised learning in credit card fraud detection - ScienceDirect</t>
+  </si>
+  <si>
+    <t>Combining unsupervised and supervised learning in credit card fraud detection</t>
+  </si>
+  <si>
+    <t>Using generative adversarial networks for improving classification effectiveness in credit card fraud detection - ScienceDirect</t>
+  </si>
+  <si>
+    <t>Using generative adversarial networks for improving classification effectiveness in credit card fraud detection</t>
   </si>
 </sst>
 </file>
@@ -244,7 +267,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -295,6 +317,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -613,163 +638,164 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024CE55D-A15F-47E0-A807-6EF1A84524AF}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="49.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="12" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="49.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6">
+        <v>2018</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="6">
+        <v>2017</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="6">
+        <v>2018</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="6">
+        <v>2017</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="10" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="7">
-        <v>2018</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="7">
-        <v>2017</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="7">
-        <v>2018</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="7">
-        <v>2017</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
     </row>
@@ -792,7 +818,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,165 +831,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="7">
+        <v>2019</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="7">
+        <v>2016</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="7">
+        <v>2019</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="7">
+        <v>2020</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="7">
+        <v>2020</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="8">
-        <v>2019</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="8">
-        <v>2016</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="8">
-        <v>2019</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="17" t="s">
+      <c r="B7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="7">
+        <v>2017</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="8">
-        <v>2020</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
-        <v>5</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="8">
-        <v>2020</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="8">
-        <v>2017</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="14"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="14"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G10" s="14"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G11" s="14"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G12" s="14"/>
+      <c r="G12" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -973,147 +999,156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3720ED4-33E9-47B9-9711-FD714142C9BB}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="7">
+        <v>2019</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="7">
+        <v>2019</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="7">
+        <v>2018</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="7">
+        <v>2019</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="7"/>
+      <c r="B6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="7">
+        <v>2017</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://ieeexplore.ieee.org/abstract/document/8717766" xr:uid="{3CC89895-74B2-4999-A54B-0F96D1A36494}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://ieeexplore.ieee.org/abstract/document/8123782" xr:uid="{214A22CE-4CFF-4A43-AFA1-212F3946BB76}"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://ieeexplore.ieee.org/abstract/document/8361343/" xr:uid="{68DCA4B0-930B-40E1-BFC8-3CB1CA0F5538}"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://www.sciencedirect.com/science/article/abs/pii/S0020025519304451" xr:uid="{072083E2-1183-420B-969A-7DCDF804EE7E}"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://www.sciencedirect.com/science/article/abs/pii/S0020025517311519" xr:uid="{49C4F4E4-9D50-40A9-BB78-E6D339EB1072}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C515C77-8D1A-4C62-AEAE-1ECF2C0C8548}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>